<commit_message>
Added html selector list for getEbayPrice
</commit_message>
<xml_diff>
--- a/ProductPriceComparison/NewWatchList.xlsx
+++ b/ProductPriceComparison/NewWatchList.xlsx
@@ -401,17 +401,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="38" customWidth="1" min="1" max="1"/>
-    <col width="35.140625" customWidth="1" min="2" max="2"/>
-    <col width="18.5703125" customWidth="1" min="3" max="3"/>
+    <col width="35.140625" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -422,12 +421,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Ebay URL</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Price</t>
         </is>
       </c>
     </row>
@@ -437,21 +436,38 @@
           <t>VisionTek RX 480 8GB GDDR5 Overclocked Edition Rear Blower 4M (3x DP, HDMI)</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>US $348.00</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>https://www.ebay.com/itm/VisionTek-RX-480-8GB-GDDR5-Overclocked-Edition-Rear-Blower-4M-3x-DP-HDMI/114683471280?hash=item1ab3aae5b0:g:aqoAAOSwK1tgKFVK</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>US $348.00</t>
+    </row>
+    <row r="3">
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>https://www.ebay.com/itm/nvidia-rtx-3060-ti-founders-edition/203288698285?hash=item2f54f35dad:g:gLkAAOSwraBgNu-p</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>https://www.ebay.com/itm/NVIDIA-GeForce-RTX-2080-Ti-Cyberpunk-2077-Edition-Front-Back-Plate-Only-USED/174648293981?_trkparms=aid%3D1110006%26algo%3DHOMESPLICE.SIM%26ao%3D1%26asc%3D230925%26meid%3D43882e1369e9447d8cea1e7aebe460c6%26pid%3D101195%26rk%3D2%26rkt%3D12%26mehot%3Dpf%26sd%3D203288698285%26itm%3D174648293981%26pmt%3D1%26noa%3D0%26pg%3D2047675%26algv%3DSimplAMLv9PairwiseUnbiasedWeb%26brand%3DNVIDIA&amp;_trksid=p2047675.c101195.m1851</t>
         </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" display="https://www.ebay.com/itm/NVIDIA-GeForce-RTX-2080-Ti-Cyberpunk-2077-Edition-Front-Back-Plate-Only-USED/174648293981?_trkparms=aid%3D1110006%26algo%3DHOMESPLICE.SIM%26ao%3D1%26asc%3D230925%26meid%3D43882e1369e9447d8cea1e7aebe460c6%26pid%3D101195%26rk%3D2%26rkt%3D12%26mehot%3Dpf%26sd%3D203288698285%26itm%3D174648293981%26pmt%3D1%26noa%3D0%26pg%3D2047675%26algv%3DSimplAMLv9PairwiseUnbiasedWeb%26brand%3DNVIDIA&amp;_trksid=p2047675.c101195.m1851" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>
 </worksheet>
 </file>
</xml_diff>